<commit_message>
game 13 in the books
</commit_message>
<xml_diff>
--- a/boardgames/seafall/captains_log/captain_kyle/province_log.xlsx
+++ b/boardgames/seafall/captains_log/captain_kyle/province_log.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="18">
   <si>
     <t>game_number</t>
   </si>
@@ -884,10 +884,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:J14"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1247,6 +1247,35 @@
         <v>16</v>
       </c>
     </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15">
+        <v>7</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="F15" t="s">
+        <v>17</v>
+      </c>
+      <c r="G15">
+        <v>6</v>
+      </c>
+      <c r="H15">
+        <v>6</v>
+      </c>
+      <c r="I15" t="s">
+        <v>12</v>
+      </c>
+      <c r="J15" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>